<commit_message>
truck tussen 8 en 10
</commit_message>
<xml_diff>
--- a/Instances/E_EGS-r.xlsx
+++ b/Instances/E_EGS-r.xlsx
@@ -1,38 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joepl\PycharmProjects\BEP_try_3.0\Instances\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/07ed5a09c14e9223/BEP/Bestanden Bilge/Instances (Synchromodal transport planning with flexible services Mathematical model and heuristic approach)/Instances/6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E38B12-5A3A-4583-BF44-C47CE89A4279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="343" documentId="11_7BAE928675DC6F2AE1E85D869446E9E15426D3EB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C632FD5B-109C-4D78-B26A-EFCD4FDAD3D1}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" tabRatio="773" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="All_vehicles" sheetId="13" r:id="rId1"/>
+    <sheet name="Allv" sheetId="13" r:id="rId1"/>
     <sheet name="Barge" sheetId="1" r:id="rId2"/>
     <sheet name="Train" sheetId="2" r:id="rId3"/>
     <sheet name="Truck" sheetId="3" r:id="rId4"/>
     <sheet name="All" sheetId="5" r:id="rId5"/>
     <sheet name="N" sheetId="7" r:id="rId6"/>
-    <sheet name="N_All" sheetId="14" r:id="rId7"/>
-    <sheet name="T" sheetId="8" r:id="rId8"/>
-    <sheet name="K" sheetId="11" r:id="rId9"/>
-    <sheet name="o" sheetId="9" r:id="rId10"/>
-    <sheet name="R_5" sheetId="12" r:id="rId11"/>
+    <sheet name="T" sheetId="8" r:id="rId7"/>
+    <sheet name="K" sheetId="11" r:id="rId8"/>
+    <sheet name="o" sheetId="9" r:id="rId9"/>
+    <sheet name="R_5" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="181">
   <si>
     <t>N</t>
   </si>
@@ -583,12 +585,6 @@
   </si>
   <si>
     <t>Nuremberg2</t>
-  </si>
-  <si>
-    <t>N_All</t>
-  </si>
-  <si>
-    <t>All</t>
   </si>
 </sst>
 </file>
@@ -983,18 +979,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB1FB023-00AF-42EC-8246-9383238A84C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08B3DF2-82A0-4881-AD66-16B5290971D2}">
   <dimension ref="A1:AE31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AC33" sqref="AC33"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Z34" sqref="Z34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3743,8 +3742,8 @@
       <c r="AD29" s="2">
         <v>1000000</v>
       </c>
-      <c r="AE29" s="2">
-        <v>1000000</v>
+      <c r="AE29">
+        <v>393.65040000000005</v>
       </c>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.25">
@@ -3927,8 +3926,8 @@
       <c r="AB31" s="2">
         <v>1000000</v>
       </c>
-      <c r="AC31" s="2">
-        <v>1000000</v>
+      <c r="AC31">
+        <v>393.65040000000005</v>
       </c>
       <c r="AD31" s="2">
         <v>1000000</v>
@@ -3943,1308 +3942,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED47BDEC-8BD7-4D64-846E-57A2265346D3}">
-  <dimension ref="A1:C117"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>57</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" t="s">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>69</v>
-      </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>70</v>
-      </c>
-      <c r="B43" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" t="s">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" t="s">
-        <v>3</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" t="s">
-        <v>4</v>
-      </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49" t="s">
-        <v>4</v>
-      </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" t="s">
-        <v>6</v>
-      </c>
-      <c r="C50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>82</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>83</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>85</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>86</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1</v>
-      </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>87</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>88</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1</v>
-      </c>
-      <c r="C58" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>89</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>90</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>91</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>92</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>93</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>94</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>95</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>96</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>97</v>
-      </c>
-      <c r="B67" t="s">
-        <v>2</v>
-      </c>
-      <c r="C67" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>98</v>
-      </c>
-      <c r="B68" t="s">
-        <v>2</v>
-      </c>
-      <c r="C68" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>99</v>
-      </c>
-      <c r="B69" t="s">
-        <v>2</v>
-      </c>
-      <c r="C69" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>100</v>
-      </c>
-      <c r="B70" t="s">
-        <v>2</v>
-      </c>
-      <c r="C70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>101</v>
-      </c>
-      <c r="B71" t="s">
-        <v>2</v>
-      </c>
-      <c r="C71" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>102</v>
-      </c>
-      <c r="B72" t="s">
-        <v>2</v>
-      </c>
-      <c r="C72" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>103</v>
-      </c>
-      <c r="B73" t="s">
-        <v>2</v>
-      </c>
-      <c r="C73" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>104</v>
-      </c>
-      <c r="B74" t="s">
-        <v>3</v>
-      </c>
-      <c r="C74" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>105</v>
-      </c>
-      <c r="B75" t="s">
-        <v>3</v>
-      </c>
-      <c r="C75" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>106</v>
-      </c>
-      <c r="B76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C76" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>107</v>
-      </c>
-      <c r="B77" t="s">
-        <v>4</v>
-      </c>
-      <c r="C77" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>108</v>
-      </c>
-      <c r="B78" t="s">
-        <v>4</v>
-      </c>
-      <c r="C78" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>109</v>
-      </c>
-      <c r="B79" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>110</v>
-      </c>
-      <c r="B80" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>111</v>
-      </c>
-      <c r="B81" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>112</v>
-      </c>
-      <c r="B82" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>113</v>
-      </c>
-      <c r="B83" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>114</v>
-      </c>
-      <c r="B84" t="s">
-        <v>1</v>
-      </c>
-      <c r="C84" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>118</v>
-      </c>
-      <c r="B85" t="s">
-        <v>1</v>
-      </c>
-      <c r="C85" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>119</v>
-      </c>
-      <c r="B86" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>120</v>
-      </c>
-      <c r="B87" t="s">
-        <v>1</v>
-      </c>
-      <c r="C87" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>121</v>
-      </c>
-      <c r="B88" t="s">
-        <v>1</v>
-      </c>
-      <c r="C88" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>122</v>
-      </c>
-      <c r="B89" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>123</v>
-      </c>
-      <c r="B90" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>124</v>
-      </c>
-      <c r="B91" t="s">
-        <v>1</v>
-      </c>
-      <c r="C91" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>125</v>
-      </c>
-      <c r="B92" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>126</v>
-      </c>
-      <c r="B93" t="s">
-        <v>2</v>
-      </c>
-      <c r="C93" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>127</v>
-      </c>
-      <c r="B94" t="s">
-        <v>2</v>
-      </c>
-      <c r="C94" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>128</v>
-      </c>
-      <c r="B95" t="s">
-        <v>2</v>
-      </c>
-      <c r="C95" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>129</v>
-      </c>
-      <c r="B96" t="s">
-        <v>2</v>
-      </c>
-      <c r="C96" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>130</v>
-      </c>
-      <c r="B97" t="s">
-        <v>2</v>
-      </c>
-      <c r="C97" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>131</v>
-      </c>
-      <c r="B98" t="s">
-        <v>2</v>
-      </c>
-      <c r="C98" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>132</v>
-      </c>
-      <c r="B99" t="s">
-        <v>2</v>
-      </c>
-      <c r="C99" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>133</v>
-      </c>
-      <c r="B100" t="s">
-        <v>2</v>
-      </c>
-      <c r="C100" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>134</v>
-      </c>
-      <c r="B101" t="s">
-        <v>3</v>
-      </c>
-      <c r="C101" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>135</v>
-      </c>
-      <c r="B102" t="s">
-        <v>3</v>
-      </c>
-      <c r="C102" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>136</v>
-      </c>
-      <c r="B103" t="s">
-        <v>3</v>
-      </c>
-      <c r="C103" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>137</v>
-      </c>
-      <c r="B104" t="s">
-        <v>3</v>
-      </c>
-      <c r="C104" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>138</v>
-      </c>
-      <c r="B105" t="s">
-        <v>3</v>
-      </c>
-      <c r="C105" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>139</v>
-      </c>
-      <c r="B106" t="s">
-        <v>3</v>
-      </c>
-      <c r="C106" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>140</v>
-      </c>
-      <c r="B107" t="s">
-        <v>3</v>
-      </c>
-      <c r="C107" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>141</v>
-      </c>
-      <c r="B108" t="s">
-        <v>4</v>
-      </c>
-      <c r="C108" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>142</v>
-      </c>
-      <c r="B109" t="s">
-        <v>4</v>
-      </c>
-      <c r="C109" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>143</v>
-      </c>
-      <c r="B110" t="s">
-        <v>4</v>
-      </c>
-      <c r="C110" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>144</v>
-      </c>
-      <c r="B111" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>145</v>
-      </c>
-      <c r="B112" t="s">
-        <v>5</v>
-      </c>
-      <c r="C112" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>146</v>
-      </c>
-      <c r="B113" t="s">
-        <v>5</v>
-      </c>
-      <c r="C113" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>147</v>
-      </c>
-      <c r="B114" t="s">
-        <v>5</v>
-      </c>
-      <c r="C114" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>148</v>
-      </c>
-      <c r="B115" t="s">
-        <v>6</v>
-      </c>
-      <c r="C115" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>149</v>
-      </c>
-      <c r="B116" t="s">
-        <v>6</v>
-      </c>
-      <c r="C116" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>150</v>
-      </c>
-      <c r="B117" t="s">
-        <v>6</v>
-      </c>
-      <c r="C117" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C81619-2CB3-4205-9A1B-A2F4AB9AA2E4}">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -5401,15 +4098,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView zoomScale="72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.625" customWidth="1"/>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="2" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" customWidth="1"/>
+    <col min="5" max="11" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -5626,21 +4324,11 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>54.911999999999999</v>
-      </c>
-      <c r="C7" s="2">
-        <v>56.628</v>
-      </c>
-      <c r="D7" s="2">
-        <v>53.195999999999998</v>
-      </c>
-      <c r="E7" s="2">
-        <v>41.183999999999997</v>
-      </c>
-      <c r="F7" s="2">
-        <v>228800000</v>
-      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="2">
         <v>0</v>
       </c>
@@ -5661,21 +4349,11 @@
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>37.752000000000002</v>
-      </c>
-      <c r="C8" s="2">
-        <v>39.468000000000004</v>
-      </c>
-      <c r="D8" s="2">
-        <v>36.036000000000001</v>
-      </c>
-      <c r="E8" s="2">
-        <v>228800000</v>
-      </c>
-      <c r="F8" s="2">
-        <v>228800000</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="2">
         <v>228800000</v>
       </c>
@@ -5696,21 +4374,11 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>58.344000000000001</v>
-      </c>
-      <c r="C9" s="2">
-        <v>60.06</v>
-      </c>
-      <c r="D9" s="2">
-        <v>228800000</v>
-      </c>
-      <c r="E9" s="2">
-        <v>228800000</v>
-      </c>
-      <c r="F9" s="2">
-        <v>228800000</v>
-      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="2">
         <v>8.58</v>
       </c>
@@ -5731,21 +4399,11 @@
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>228800000</v>
-      </c>
-      <c r="C10" s="2">
-        <v>228800000</v>
-      </c>
-      <c r="D10" s="2">
-        <v>228800000</v>
-      </c>
-      <c r="E10" s="2">
-        <v>228800000</v>
-      </c>
-      <c r="F10" s="2">
-        <v>228800000</v>
-      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="2">
         <v>228800000</v>
       </c>
@@ -5808,7 +4466,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -6212,7 +4870,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:K11"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -6619,8 +5277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -7027,7 +5685,7 @@
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -7093,18 +5751,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8153B036-FE5E-4DC3-979D-FBA930CA6D11}">
-  <dimension ref="A1:A31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7D789-45BF-49AF-B085-C0D33A463D09}">
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -7155,106 +5811,6 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -7263,79 +5819,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F7D789-45BF-49AF-B085-C0D33A463D09}">
-  <dimension ref="A1:A11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA89C9B-3D6A-45B9-B7D6-07F0C8919DAB}">
+  <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA89C9B-3D6A-45B9-B7D6-07F0C8919DAB}">
-  <dimension ref="A1:G118"/>
-  <sheetViews>
-    <sheetView topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -10031,27 +8519,1306 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>182</v>
-      </c>
-      <c r="B118">
-        <v>1</v>
-      </c>
-      <c r="C118">
-        <v>1</v>
-      </c>
-      <c r="D118">
-        <v>1</v>
-      </c>
-      <c r="E118">
-        <v>1</v>
-      </c>
-      <c r="F118">
-        <v>1</v>
-      </c>
-      <c r="G118">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED47BDEC-8BD7-4D64-846E-57A2265346D3}">
+  <dimension ref="A1:C117"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>74</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4</v>
+      </c>
+      <c r="C48" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>87</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>88</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>89</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>92</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>93</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>94</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>95</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>97</v>
+      </c>
+      <c r="B67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>99</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>101</v>
+      </c>
+      <c r="B71" t="s">
+        <v>2</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>102</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>103</v>
+      </c>
+      <c r="B73" t="s">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>104</v>
+      </c>
+      <c r="B74" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>105</v>
+      </c>
+      <c r="B75" t="s">
+        <v>3</v>
+      </c>
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>106</v>
+      </c>
+      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>107</v>
+      </c>
+      <c r="B77" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>108</v>
+      </c>
+      <c r="B78" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>109</v>
+      </c>
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>110</v>
+      </c>
+      <c r="B80" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>111</v>
+      </c>
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>112</v>
+      </c>
+      <c r="B82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>113</v>
+      </c>
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>114</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>118</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>119</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>120</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1</v>
+      </c>
+      <c r="C88" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>122</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>123</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>124</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>125</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>126</v>
+      </c>
+      <c r="B93" t="s">
+        <v>2</v>
+      </c>
+      <c r="C93" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>127</v>
+      </c>
+      <c r="B94" t="s">
+        <v>2</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>128</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>129</v>
+      </c>
+      <c r="B96" t="s">
+        <v>2</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>130</v>
+      </c>
+      <c r="B97" t="s">
+        <v>2</v>
+      </c>
+      <c r="C97" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>131</v>
+      </c>
+      <c r="B98" t="s">
+        <v>2</v>
+      </c>
+      <c r="C98" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>132</v>
+      </c>
+      <c r="B99" t="s">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>133</v>
+      </c>
+      <c r="B100" t="s">
+        <v>2</v>
+      </c>
+      <c r="C100" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>134</v>
+      </c>
+      <c r="B101" t="s">
+        <v>3</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>135</v>
+      </c>
+      <c r="B102" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>136</v>
+      </c>
+      <c r="B103" t="s">
+        <v>3</v>
+      </c>
+      <c r="C103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>137</v>
+      </c>
+      <c r="B104" t="s">
+        <v>3</v>
+      </c>
+      <c r="C104" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>138</v>
+      </c>
+      <c r="B105" t="s">
+        <v>3</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>139</v>
+      </c>
+      <c r="B106" t="s">
+        <v>3</v>
+      </c>
+      <c r="C106" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>140</v>
+      </c>
+      <c r="B107" t="s">
+        <v>3</v>
+      </c>
+      <c r="C107" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>141</v>
+      </c>
+      <c r="B108" t="s">
+        <v>4</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>142</v>
+      </c>
+      <c r="B109" t="s">
+        <v>4</v>
+      </c>
+      <c r="C109" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>143</v>
+      </c>
+      <c r="B110" t="s">
+        <v>4</v>
+      </c>
+      <c r="C110" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>144</v>
+      </c>
+      <c r="B111" t="s">
+        <v>5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>145</v>
+      </c>
+      <c r="B112" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>146</v>
+      </c>
+      <c r="B113" t="s">
+        <v>5</v>
+      </c>
+      <c r="C113" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>147</v>
+      </c>
+      <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>148</v>
+      </c>
+      <c r="B115" t="s">
+        <v>6</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>149</v>
+      </c>
+      <c r="B116" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>150</v>
+      </c>
+      <c r="B117" t="s">
+        <v>6</v>
+      </c>
+      <c r="C117" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>